<commit_message>
Update BOM excel file
</commit_message>
<xml_diff>
--- a/ESP8266/BOM.xlsx
+++ b/ESP8266/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tuann\OneDrive\Desktop\WS2812B-LED-LAMP\ESP8266\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21653C25-968F-4BA8-8463-5D5698F3A794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593908E7-C744-4F36-8C2D-DC5369E17D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>No.</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Mạch Hiển Thị 4 Led 7 Đoạn TM1637 (kiểu thời gian)</t>
+  </si>
+  <si>
+    <t>Mạch WS2812B ma trận 8*8</t>
   </si>
 </sst>
 </file>
@@ -96,11 +99,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,13 +397,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -445,10 +448,21 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
     </row>

</xml_diff>